<commit_message>
Update Laporan_Keuangan.pdf with revised financial data
</commit_message>
<xml_diff>
--- a/src/Laporan_Keuangan.xlsx
+++ b/src/Laporan_Keuangan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Pendataan-Desa\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8D73CE-001D-4620-B131-9ACF710E759B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233A678A-37EB-4E5D-9662-2AF09440D88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{434B3040-041E-43FD-AB34-AECA2D945A56}"/>
   </bookViews>
@@ -507,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -601,20 +601,59 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -622,44 +661,8 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -677,6 +680,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>826978</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>153580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>41349</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>13054</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5E6A432-0F99-DD52-29A4-FC39FB157FC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3278373" y="537533"/>
+          <a:ext cx="3626883" cy="2163195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -981,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="129" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1001,28 +1059,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
     </row>
     <row r="2" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G2" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="47">
+      <c r="H2" s="52">
         <v>45399</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1041,8 +1099,13 @@
         <v>96</v>
       </c>
       <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="J4" s="31"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -1052,8 +1115,13 @@
         <v>98</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
     </row>
     <row r="6" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -1063,8 +1131,13 @@
         <v>56</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
@@ -1074,7 +1147,13 @@
         <v>47</v>
       </c>
       <c r="C7" s="31"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
@@ -1084,7 +1163,13 @@
         <v>49</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
@@ -1094,19 +1179,37 @@
         <v>51</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
@@ -1116,7 +1219,13 @@
         <v>102</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
@@ -1126,13 +1235,25 @@
         <v>103</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -1141,12 +1262,12 @@
       <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -1160,10 +1281,10 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="14" t="s">
         <v>75</v>
       </c>
@@ -1171,19 +1292,19 @@
         <v>100</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="14" t="s">
         <v>76</v>
       </c>
@@ -1191,21 +1312,21 @@
         <v>60</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="42"/>
+      <c r="G19" s="39"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="39">
+      <c r="I19" s="40">
         <v>0.05</v>
       </c>
-      <c r="J19" s="39"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="37"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="23" t="s">
         <v>78</v>
       </c>
@@ -1213,15 +1334,15 @@
         <v>59</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="42"/>
+      <c r="G20" s="39"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="40"/>
     </row>
     <row r="21" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -1240,17 +1361,17 @@
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="26"/>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="41"/>
+      <c r="J21" s="54"/>
       <c r="P21" s="6"/>
     </row>
     <row r="22" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="37"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="22" t="s">
         <v>77</v>
       </c>
@@ -1263,18 +1384,18 @@
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="27"/>
-      <c r="I22" s="45" t="s">
+      <c r="I22" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="J22" s="38"/>
+      <c r="J22" s="41"/>
       <c r="O22" s="5"/>
       <c r="P22" s="6"/>
     </row>
     <row r="23" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="14" t="s">
         <v>79</v>
       </c>
@@ -1282,10 +1403,10 @@
         <v>62</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="53"/>
       <c r="H23" s="28" t="s">
         <v>21</v>
       </c>
@@ -1297,10 +1418,10 @@
       <c r="P23" s="6"/>
     </row>
     <row r="24" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="37"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="22" t="s">
         <v>80</v>
       </c>
@@ -1308,10 +1429,10 @@
         <v>63</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="48" t="s">
+      <c r="F24" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="48"/>
+      <c r="G24" s="36"/>
       <c r="H24" s="28" t="s">
         <v>21</v>
       </c>
@@ -1321,10 +1442,10 @@
       <c r="J24" s="46"/>
     </row>
     <row r="25" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="37"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="22" t="s">
         <v>81</v>
       </c>
@@ -1339,16 +1460,16 @@
       <c r="H25" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="38" t="s">
+      <c r="I25" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="38"/>
+      <c r="J25" s="41"/>
     </row>
     <row r="26" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="37"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="14" t="s">
         <v>82</v>
       </c>
@@ -1356,23 +1477,23 @@
         <v>65</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="48"/>
+      <c r="G26" s="36"/>
       <c r="H26" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="38" t="s">
+      <c r="I26" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="38"/>
+      <c r="J26" s="41"/>
     </row>
     <row r="27" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="37"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="14" t="s">
         <v>83</v>
       </c>
@@ -1380,23 +1501,23 @@
         <v>66</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="48"/>
+      <c r="G27" s="36"/>
       <c r="H27" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="38" t="s">
+      <c r="I27" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="J27" s="38"/>
+      <c r="J27" s="41"/>
     </row>
     <row r="28" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="37"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="14" t="s">
         <v>84</v>
       </c>
@@ -1404,23 +1525,23 @@
         <v>67</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="48" t="s">
+      <c r="F28" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="48"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="38" t="s">
+      <c r="I28" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="38"/>
+      <c r="J28" s="41"/>
     </row>
     <row r="29" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="37"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="29" t="s">
         <v>85</v>
       </c>
@@ -1428,21 +1549,21 @@
         <v>68</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="48"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="24"/>
-      <c r="I29" s="51">
+      <c r="I29" s="43">
         <v>0.05</v>
       </c>
-      <c r="J29" s="51"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="37"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="22" t="s">
         <v>86</v>
       </c>
@@ -1450,23 +1571,23 @@
         <v>69</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="48"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I30" s="53" t="s">
+      <c r="I30" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="J30" s="52"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="37"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="22" t="s">
         <v>87</v>
       </c>
@@ -1481,10 +1602,10 @@
       <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="37"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="22" t="s">
         <v>92</v>
       </c>
@@ -1492,19 +1613,19 @@
         <v>71</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="50" t="s">
+      <c r="F32" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
     </row>
     <row r="33" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="37"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="22" t="s">
         <v>88</v>
       </c>
@@ -1515,18 +1636,18 @@
       <c r="F33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
     </row>
     <row r="34" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="37"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="22" t="s">
         <v>89</v>
       </c>
@@ -1535,16 +1656,16 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="24"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
     </row>
     <row r="35" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="37"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="22" t="s">
         <v>90</v>
       </c>
@@ -1555,18 +1676,18 @@
       <c r="F35" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="35" t="s">
+      <c r="G35" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
     </row>
     <row r="36" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="14" t="s">
         <v>91</v>
       </c>
@@ -1576,34 +1697,68 @@
       <c r="F36" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="G36" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="54"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="22" t="s">
         <v>105</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="35" t="s">
+      <c r="G37" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="50">
+    <mergeCell ref="G33:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D4:J14"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="G36:J36"/>
     <mergeCell ref="G37:J37"/>
@@ -1620,42 +1775,10 @@
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="I24:J24"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="G33:J34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.3" right="0.25" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="98" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>